<commit_message>
update excel - hmk 1,2
</commit_message>
<xml_diff>
--- a/metodosnum2020.xlsx
+++ b/metodosnum2020.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="127">
   <si>
     <t>Estrella de Alhely Hernández Mérida</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>https://github.com/martinhernandezjuarez/martinhernandez</t>
+  </si>
+  <si>
+    <t>se deben subir los .m</t>
   </si>
 </sst>
 </file>
@@ -2722,10 +2725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2736,7 +2739,7 @@
     <col min="9" max="9" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="E1" s="3" t="s">
         <v>86</v>
       </c>
@@ -2753,7 +2756,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2770,10 +2773,10 @@
         <v>110</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -2782,7 +2785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2798,9 +2801,20 @@
       <c r="E4" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2817,19 +2831,19 @@
         <v>108</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I5" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2846,19 +2860,22 @@
         <v>115</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="4">
         <v>0</v>
       </c>
+      <c r="J6" t="s">
+        <v>126</v>
+      </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2875,19 +2892,19 @@
         <v>96</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2903,9 +2920,20 @@
       <c r="E8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2922,19 +2950,19 @@
         <v>99</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2951,19 +2979,19 @@
         <v>93</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2980,19 +3008,19 @@
         <v>102</v>
       </c>
       <c r="F11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3009,19 +3037,19 @@
         <v>107</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3038,19 +3066,19 @@
         <v>98</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3067,19 +3095,19 @@
         <v>112</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3095,9 +3123,20 @@
       <c r="E15" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3143,13 +3182,13 @@
         <v>91</v>
       </c>
       <c r="F17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="4">
         <v>0</v>
@@ -3171,7 +3210,18 @@
       <c r="E18" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1">
@@ -3196,7 +3246,7 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I19" s="4">
         <v>0</v>
@@ -3219,13 +3269,13 @@
         <v>113</v>
       </c>
       <c r="F20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="4">
         <v>0</v>
@@ -3247,7 +3297,18 @@
       <c r="E21" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1">
@@ -3266,13 +3327,13 @@
         <v>103</v>
       </c>
       <c r="F22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="4">
         <v>0</v>
@@ -3294,7 +3355,18 @@
       <c r="E23" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1">
@@ -3313,13 +3385,13 @@
         <v>104</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="4">
         <v>0</v>
@@ -3342,13 +3414,13 @@
         <v>101</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="4">
         <v>0</v>
@@ -3371,13 +3443,13 @@
         <v>85</v>
       </c>
       <c r="F26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="4">
         <v>0</v>
@@ -3400,13 +3472,13 @@
         <v>92</v>
       </c>
       <c r="F27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I27" s="4">
         <v>0</v>
@@ -3429,13 +3501,13 @@
         <v>87</v>
       </c>
       <c r="F28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="5">
         <v>0</v>
@@ -3458,13 +3530,13 @@
         <v>105</v>
       </c>
       <c r="F29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="4">
         <v>0</v>
@@ -3487,13 +3559,13 @@
         <v>118</v>
       </c>
       <c r="F30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="4">
         <v>0</v>
@@ -3545,13 +3617,13 @@
         <v>84</v>
       </c>
       <c r="F32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="4">
         <v>0</v>
@@ -3574,16 +3646,16 @@
         <v>106</v>
       </c>
       <c r="F33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I33" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -3603,10 +3675,10 @@
         <v>100</v>
       </c>
       <c r="F34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3632,13 +3704,13 @@
         <v>121</v>
       </c>
       <c r="F35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="4">
         <v>0</v>
@@ -3690,13 +3762,13 @@
         <v>114</v>
       </c>
       <c r="F37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="4">
         <v>0</v>
@@ -3719,13 +3791,13 @@
         <v>109</v>
       </c>
       <c r="F38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
add w3 - secante
</commit_message>
<xml_diff>
--- a/metodosnum2020.xlsx
+++ b/metodosnum2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="6160" yWindow="1680" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2727,8 +2727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
add w7 ses 2
</commit_message>
<xml_diff>
--- a/metodosnum2020.xlsx
+++ b/metodosnum2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="2320" yWindow="20" windowWidth="25280" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -771,8 +771,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -823,8 +823,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -875,8 +875,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -927,8 +927,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -979,8 +979,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1031,8 +1031,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1083,8 +1083,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1135,8 +1135,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1187,8 +1187,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1239,8 +1239,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1291,8 +1291,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1343,8 +1343,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1395,8 +1395,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1447,8 +1447,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1499,8 +1499,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1551,8 +1551,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1603,8 +1603,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1655,8 +1655,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1707,8 +1707,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1759,8 +1759,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1811,8 +1811,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1863,8 +1863,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1915,8 +1915,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1967,8 +1967,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2019,8 +2019,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2071,8 +2071,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2123,8 +2123,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2175,8 +2175,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2227,8 +2227,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2279,8 +2279,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2331,8 +2331,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2383,8 +2383,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2435,8 +2435,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2487,8 +2487,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2539,8 +2539,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2591,8 +2591,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2643,8 +2643,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -3014,17 +3014,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="Z22" sqref="Z22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="1.5" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="1.83203125" customWidth="1"/>
     <col min="4" max="4" width="0.6640625" customWidth="1"/>
     <col min="6" max="6" width="12" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="5"/>
+    <col min="7" max="7" width="1.83203125" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="9" max="9" width="2.5" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="3.1640625" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" customWidth="1"/>
     <col min="13" max="13" width="3.6640625" customWidth="1"/>
     <col min="14" max="14" width="2.6640625" customWidth="1"/>
     <col min="15" max="15" width="6.33203125" style="21" customWidth="1"/>

</xml_diff>

<commit_message>
add w11 - sess 2
</commit_message>
<xml_diff>
--- a/metodosnum2020.xlsx
+++ b/metodosnum2020.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="177">
   <si>
     <t>Estrella de Alhely Hernández Mérida</t>
   </si>
@@ -549,6 +549,9 @@
   </si>
   <si>
     <t>https://github.com/Caro0602/CarolinaCruzFlores_parcial2</t>
+  </si>
+  <si>
+    <t>https://github.com/miguel-lv/MiguelAngelLopezVieyra_Parcial_2</t>
   </si>
 </sst>
 </file>
@@ -10551,8 +10554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12163,7 +12166,7 @@
         <v>130</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="G20">
         <v>0</v>

</xml_diff>